<commit_message>
[reader] added tests for common types
</commit_message>
<xml_diff>
--- a/src/openpyxl/tests/test_data/genuine/empty-with-styles.xlsx
+++ b/src/openpyxl/tests/test_data/genuine/empty-with-styles.xlsx
@@ -52,11 +52,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,7 +374,7 @@
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>3.14</v>
       </c>
     </row>

</xml_diff>